<commit_message>
Updating the 2025 year plan
</commit_message>
<xml_diff>
--- a/Missing sites on 2023 list.xlsx
+++ b/Missing sites on 2023 list.xlsx
@@ -8,17 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atconline-my.sharepoint.com/personal/allan_kavuma_americantower_com/Documents/Documents/SDM 2019/Analysis/2023 SDS Site Allocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC1048D0A91D6F2C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96F7E8E0-3390-47B4-9A9F-BA55DDED5088}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048D0A91D6F2C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4808FA5-6FFD-487F-B131-5BBA5F0AFEC9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="384" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1372,7 +1386,7 @@
   <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A1:F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4056,6 +4070,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="8" priority="8"/>
     <cfRule type="duplicateValues" dxfId="7" priority="9"/>

</xml_diff>